<commit_message>
Añadida la altura y el peso de los pokemon al excel
</commit_message>
<xml_diff>
--- a/ST/Data/web/poke_info.xlsx
+++ b/ST/Data/web/poke_info.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40809_{04268BAA-2A2E-408C-B703-8AE0967E015D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A8325296-1655-4909-B5AA-C1A6842B7320}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14980" windowHeight="11060"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="15020" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="poke_info" sheetId="1" r:id="rId1"/>
@@ -174,11 +174,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -201,8 +207,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,11 +523,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -528,7 +535,7 @@
     <col min="1" max="256" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -550,8 +557,14 @@
       <c r="H2">
         <v>219</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J2">
+        <v>135.5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -573,8 +586,14 @@
       <c r="H3">
         <v>219</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1.7</v>
+      </c>
+      <c r="J3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -596,8 +615,14 @@
       <c r="H4">
         <v>199</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>2.1</v>
+      </c>
+      <c r="J4">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -619,8 +644,14 @@
       <c r="H5">
         <v>215</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>2.7</v>
+      </c>
+      <c r="J5">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -642,8 +673,14 @@
       <c r="H6">
         <v>219</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>2.1</v>
+      </c>
+      <c r="J6">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -665,8 +702,14 @@
       <c r="H7">
         <v>259</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>1.9</v>
+      </c>
+      <c r="J7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -688,8 +731,14 @@
       <c r="H8">
         <v>165</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1.3</v>
+      </c>
+      <c r="J8">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -711,8 +760,14 @@
       <c r="H9">
         <v>259</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>34.299999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -734,8 +789,14 @@
       <c r="H10">
         <v>299</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>1.7</v>
+      </c>
+      <c r="J10">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -757,8 +818,14 @@
       <c r="H11">
         <v>239</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>1.5</v>
+      </c>
+      <c r="J11">
+        <v>132.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -780,8 +847,14 @@
       <c r="H12">
         <v>259</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J12">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -803,8 +876,14 @@
       <c r="H13">
         <v>199</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>2.1</v>
+      </c>
+      <c r="J13">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -826,8 +905,14 @@
       <c r="H14">
         <v>319</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>0.9</v>
+      </c>
+      <c r="J14">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -849,8 +934,14 @@
       <c r="H15">
         <v>329</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J15">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -872,8 +963,14 @@
       <c r="H16">
         <v>299</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -895,8 +992,14 @@
       <c r="H17">
         <v>319</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>1.3</v>
+      </c>
+      <c r="J17">
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -918,8 +1021,14 @@
       <c r="H18">
         <v>259</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>1.6</v>
+      </c>
+      <c r="J18">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -941,8 +1050,14 @@
       <c r="H19">
         <v>315</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>0.8</v>
+      </c>
+      <c r="J19">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -964,8 +1079,14 @@
       <c r="H20">
         <v>303</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>1.9</v>
+      </c>
+      <c r="J20">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>19</v>
       </c>
@@ -987,8 +1108,14 @@
       <c r="H21">
         <v>259</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>1.6</v>
+      </c>
+      <c r="J21">
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -1010,8 +1137,14 @@
       <c r="H22">
         <v>319</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>1.5</v>
+      </c>
+      <c r="J22">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -1033,8 +1166,14 @@
       <c r="H23">
         <v>229</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>0.8</v>
+      </c>
+      <c r="J23">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -1056,8 +1195,14 @@
       <c r="H24">
         <v>289</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -1079,8 +1224,14 @@
       <c r="H25">
         <v>289</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>24</v>
       </c>
@@ -1102,8 +1253,14 @@
       <c r="H26">
         <v>359</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>0.8</v>
+      </c>
+      <c r="J26">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -1125,8 +1282,14 @@
       <c r="H27">
         <v>279</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>1.2</v>
+      </c>
+      <c r="J27">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>26</v>
       </c>
@@ -1148,8 +1311,14 @@
       <c r="H28">
         <v>281</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>1.2</v>
+      </c>
+      <c r="J28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>27</v>
       </c>
@@ -1171,8 +1340,14 @@
       <c r="H29">
         <v>239</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>1.4</v>
+      </c>
+      <c r="J29">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>28</v>
       </c>
@@ -1194,8 +1369,14 @@
       <c r="H30">
         <v>323</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>29</v>
       </c>
@@ -1217,8 +1398,14 @@
       <c r="H31">
         <v>219</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>1.2</v>
+      </c>
+      <c r="J31">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -1240,8 +1427,14 @@
       <c r="H32">
         <v>239</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>1.6</v>
+      </c>
+      <c r="J32">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -1263,8 +1456,14 @@
       <c r="H33">
         <v>261</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>6.2</v>
+      </c>
+      <c r="J33">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -1286,8 +1485,14 @@
       <c r="H34">
         <v>291</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>0.2</v>
+      </c>
+      <c r="J34">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>33</v>
       </c>
@@ -1309,8 +1514,14 @@
       <c r="H35">
         <v>309</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>0.9</v>
+      </c>
+      <c r="J35">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -1332,8 +1543,14 @@
       <c r="H36">
         <v>179</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>0.8</v>
+      </c>
+      <c r="J36">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>35</v>
       </c>
@@ -1355,8 +1572,14 @@
       <c r="H37">
         <v>319</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>0.7</v>
+      </c>
+      <c r="J37">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>36</v>
       </c>
@@ -1378,8 +1601,14 @@
       <c r="H38">
         <v>169</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>20.100000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>37</v>
       </c>
@@ -1401,8 +1630,14 @@
       <c r="H39">
         <v>333</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>1.2</v>
+      </c>
+      <c r="J39">
+        <v>22.2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -1424,8 +1659,14 @@
       <c r="H40">
         <v>339</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>1.7</v>
+      </c>
+      <c r="J40">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>39</v>
       </c>
@@ -1447,8 +1688,14 @@
       <c r="H41">
         <v>323</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>2.5</v>
+      </c>
+      <c r="J41">
+        <v>200.5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>40</v>
       </c>
@@ -1470,8 +1717,14 @@
       <c r="H42">
         <v>325</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>3.3</v>
+      </c>
+      <c r="J42">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>41</v>
       </c>
@@ -1493,8 +1746,14 @@
       <c r="H43">
         <v>169</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>42</v>
       </c>
@@ -1516,8 +1775,14 @@
       <c r="H44">
         <v>219</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>43</v>
       </c>
@@ -1539,8 +1804,14 @@
       <c r="H45">
         <v>259</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>1.5</v>
+      </c>
+      <c r="J45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>44</v>
       </c>
@@ -1562,8 +1833,14 @@
       <c r="H46">
         <v>299</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>1.7</v>
+      </c>
+      <c r="J46">
+        <v>79.5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>45</v>
       </c>
@@ -1585,8 +1862,14 @@
       <c r="H47">
         <v>221</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>46</v>
       </c>
@@ -1608,8 +1891,14 @@
       <c r="H48">
         <v>229</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>47</v>
       </c>
@@ -1631,8 +1920,14 @@
       <c r="H49">
         <v>229</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>48</v>
       </c>
@@ -1654,8 +1949,14 @@
       <c r="H50">
         <v>259</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>2</v>
+      </c>
+      <c r="J50">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>49</v>
       </c>
@@ -1672,13 +1973,19 @@
         <v>269</v>
       </c>
       <c r="G51">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="H51">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>50</v>
       </c>
@@ -1700,14 +2007,22 @@
       <c r="H52">
         <v>289</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25"/>
+      <c r="I52">
+        <v>1.9</v>
+      </c>
+      <c r="J52">
+        <v>51.5</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Añadidos los tipos al excel
</commit_message>
<xml_diff>
--- a/ST/Data/web/poke_info.xlsx
+++ b/ST/Data/web/poke_info.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A8325296-1655-4909-B5AA-C1A6842B7320}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B3F9382A-FB2B-417C-9C93-E18607E817AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="15020" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="15060" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="poke_info" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="70">
   <si>
     <t>Abomasnow</t>
   </si>
@@ -169,6 +169,63 @@
   </si>
   <si>
     <t>Yanmega</t>
+  </si>
+  <si>
+    <t>Planta</t>
+  </si>
+  <si>
+    <t>Hielo</t>
+  </si>
+  <si>
+    <t>Fantasma</t>
+  </si>
+  <si>
+    <t>Roca</t>
+  </si>
+  <si>
+    <t>Acero</t>
+  </si>
+  <si>
+    <t>Hiero</t>
+  </si>
+  <si>
+    <t>Lucha</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Fuego</t>
+  </si>
+  <si>
+    <t>Phiquico</t>
+  </si>
+  <si>
+    <t>Volador</t>
+  </si>
+  <si>
+    <t>Agua</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>Electrico</t>
+  </si>
+  <si>
+    <t>Siniestro</t>
+  </si>
+  <si>
+    <t>Tierra</t>
+  </si>
+  <si>
+    <t>Hada</t>
+  </si>
+  <si>
+    <t>Veneno</t>
+  </si>
+  <si>
+    <t>Bicho</t>
   </si>
 </sst>
 </file>
@@ -524,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J56"/>
+  <dimension ref="B2:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -535,7 +592,7 @@
     <col min="1" max="256" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -563,8 +620,14 @@
       <c r="J2">
         <v>135.5</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -592,8 +655,14 @@
       <c r="J3">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -621,8 +690,14 @@
       <c r="J4">
         <v>360</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -650,8 +725,14 @@
       <c r="J5">
         <v>225</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -679,8 +760,14 @@
       <c r="J6">
         <v>135</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -708,8 +795,14 @@
       <c r="J7">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -737,8 +830,14 @@
       <c r="J8">
         <v>187</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -766,8 +865,14 @@
       <c r="J9">
         <v>34.299999999999997</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -795,8 +900,14 @@
       <c r="J10">
         <v>90.5</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -824,8 +935,14 @@
       <c r="J11">
         <v>132.5</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -853,8 +970,14 @@
       <c r="J12">
         <v>210</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -882,8 +1005,11 @@
       <c r="J13">
         <v>85.5</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -911,8 +1037,11 @@
       <c r="J14">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -940,8 +1069,11 @@
       <c r="J15">
         <v>33.5</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -969,8 +1101,14 @@
       <c r="J16">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>63</v>
+      </c>
+      <c r="L16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -998,8 +1136,14 @@
       <c r="J17">
         <v>26.6</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>52</v>
+      </c>
+      <c r="L17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -1027,8 +1171,14 @@
       <c r="J18">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -1056,8 +1206,14 @@
       <c r="J19">
         <v>14.3</v>
       </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -1085,8 +1241,14 @@
       <c r="J20">
         <v>95</v>
       </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>63</v>
+      </c>
+      <c r="L20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>19</v>
       </c>
@@ -1114,8 +1276,14 @@
       <c r="J21">
         <v>48.4</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>67</v>
+      </c>
+      <c r="L21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -1143,8 +1311,14 @@
       <c r="J22">
         <v>40.5</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>68</v>
+      </c>
+      <c r="L22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -1172,8 +1346,11 @@
       <c r="J23">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -1201,8 +1378,14 @@
       <c r="J24">
         <v>42.5</v>
       </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>66</v>
+      </c>
+      <c r="L24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -1230,8 +1413,11 @@
       <c r="J25">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>24</v>
       </c>
@@ -1259,8 +1445,11 @@
       <c r="J26">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -1288,8 +1477,14 @@
       <c r="J27">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>55</v>
+      </c>
+      <c r="L27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>26</v>
       </c>
@@ -1317,8 +1512,11 @@
       <c r="J28">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>27</v>
       </c>
@@ -1346,8 +1544,11 @@
       <c r="J29">
         <v>42</v>
       </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>28</v>
       </c>
@@ -1375,8 +1576,11 @@
       <c r="J30">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>29</v>
       </c>
@@ -1404,8 +1608,14 @@
       <c r="J31">
         <v>180</v>
       </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>55</v>
+      </c>
+      <c r="L31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -1433,8 +1643,14 @@
       <c r="J32">
         <v>550</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>55</v>
+      </c>
+      <c r="L32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -1462,8 +1678,11 @@
       <c r="J33">
         <v>162</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -1491,8 +1710,14 @@
       <c r="J34">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>67</v>
+      </c>
+      <c r="L34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>33</v>
       </c>
@@ -1520,8 +1745,11 @@
       <c r="J35">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -1549,8 +1777,11 @@
       <c r="J36">
         <v>36.5</v>
       </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>35</v>
       </c>
@@ -1578,8 +1809,14 @@
       <c r="J37">
         <v>21</v>
       </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>64</v>
+      </c>
+      <c r="L37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>36</v>
       </c>
@@ -1607,8 +1844,11 @@
       <c r="J38">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>37</v>
       </c>
@@ -1636,8 +1876,14 @@
       <c r="J39">
         <v>22.2</v>
       </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>68</v>
+      </c>
+      <c r="L39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -1665,8 +1911,11 @@
       <c r="J40">
         <v>52.2</v>
       </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>39</v>
       </c>
@@ -1694,8 +1943,14 @@
       <c r="J41">
         <v>200.5</v>
       </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>69</v>
+      </c>
+      <c r="L41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>40</v>
       </c>
@@ -1723,8 +1978,11 @@
       <c r="J42">
         <v>63</v>
       </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>41</v>
       </c>
@@ -1752,8 +2010,14 @@
       <c r="J43">
         <v>108</v>
       </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K43" t="s">
+        <v>65</v>
+      </c>
+      <c r="L43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>42</v>
       </c>
@@ -1781,8 +2045,11 @@
       <c r="J44">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>43</v>
       </c>
@@ -1810,8 +2077,14 @@
       <c r="J45">
         <v>38</v>
       </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K45" t="s">
+        <v>67</v>
+      </c>
+      <c r="L45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>44</v>
       </c>
@@ -1839,8 +2112,11 @@
       <c r="J46">
         <v>79.5</v>
       </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>45</v>
       </c>
@@ -1868,8 +2144,14 @@
       <c r="J47">
         <v>202</v>
       </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
+        <v>54</v>
+      </c>
+      <c r="L47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>46</v>
       </c>
@@ -1897,8 +2179,11 @@
       <c r="J48">
         <v>27</v>
       </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>47</v>
       </c>
@@ -1926,8 +2211,11 @@
       <c r="J49">
         <v>29</v>
       </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>48</v>
       </c>
@@ -1955,8 +2243,14 @@
       <c r="J50">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>51</v>
+      </c>
+      <c r="L50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>49</v>
       </c>
@@ -1984,8 +2278,14 @@
       <c r="J51">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>58</v>
+      </c>
+      <c r="L51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>50</v>
       </c>
@@ -2013,13 +2313,19 @@
       <c r="J52">
         <v>51.5</v>
       </c>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K52" t="s">
+        <v>69</v>
+      </c>
+      <c r="L52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Leer la informacion de un excel. falta guardarla en una lista
</commit_message>
<xml_diff>
--- a/ST/Data/web/poke_info.xlsx
+++ b/ST/Data/web/poke_info.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr checkCompatibility="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{09998096-055A-46BC-A4EF-35B1FE030F1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{A7B57187-E546-43DF-B63D-2D360DB4DBCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="15180" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="15220" windowHeight="11060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="poke_info" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -358,9 +358,6 @@
     <t>Puño fuego</t>
   </si>
   <si>
-    <t>Evite ígneo</t>
-  </si>
-  <si>
     <t>Patada salto alta</t>
   </si>
   <si>
@@ -725,16 +722,26 @@
   </si>
   <si>
     <t xml:space="preserve">Espacio raro </t>
+  </si>
+  <si>
+    <t>Envite ígneo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -773,13 +780,14 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1098,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:V53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I37" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView tabSelected="1" topLeftCell="K34" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1221,7 +1229,7 @@
         <v>82</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>83</v>
@@ -1474,29 +1482,29 @@
       <c r="K7" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>102</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R7" s="2" t="s">
         <v>87</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T7" s="2" t="s">
         <v>92</v>
@@ -1537,22 +1545,22 @@
         <v>187</v>
       </c>
       <c r="K8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="N8" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>100</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>98</v>
@@ -1602,13 +1610,13 @@
         <v>34.299999999999997</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>98</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>83</v>
@@ -1617,19 +1625,19 @@
         <v>100</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="R9" s="2" t="s">
         <v>77</v>
       </c>
       <c r="S9" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="T9" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="T9" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="U9" t="s">
         <v>59</v>
@@ -1667,19 +1675,19 @@
         <v>90.5</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="L10" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="M10" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>107</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>77</v>
@@ -1688,13 +1696,13 @@
         <v>109</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S10" s="2" t="s">
         <v>87</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U10" t="s">
         <v>60</v>
@@ -1732,16 +1740,16 @@
         <v>132.5</v>
       </c>
       <c r="K11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>75</v>
@@ -1753,13 +1761,13 @@
         <v>98</v>
       </c>
       <c r="R11" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="T11" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="T11" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="U11" t="s">
         <v>61</v>
@@ -1797,19 +1805,19 @@
         <v>210</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>96</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>94</v>
@@ -1824,7 +1832,7 @@
         <v>77</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="U12" t="s">
         <v>62</v>
@@ -1862,13 +1870,13 @@
         <v>85.5</v>
       </c>
       <c r="K13" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>98</v>
@@ -1886,10 +1894,10 @@
         <v>77</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="U13" t="s">
         <v>63</v>
@@ -1927,7 +1935,7 @@
         <v>83</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>77</v>
@@ -1939,19 +1947,19 @@
         <v>100</v>
       </c>
       <c r="P14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q14" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="R14" s="2" t="s">
         <v>76</v>
       </c>
       <c r="S14" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="T14" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="U14" t="s">
         <v>64</v>
@@ -1986,34 +1994,34 @@
         <v>33.5</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L15" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="M15" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>98</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="R15" s="2" t="s">
         <v>76</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="U15" t="s">
         <v>61</v>
@@ -2048,25 +2056,25 @@
         <v>82</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>79</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>98</v>
       </c>
       <c r="O16" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="P16" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="Q16" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="R16" s="2" t="s">
         <v>76</v>
@@ -2113,16 +2121,16 @@
         <v>26.6</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>75</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>83</v>
@@ -2131,7 +2139,7 @@
         <v>96</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R17" s="2" t="s">
         <v>98</v>
@@ -2140,7 +2148,7 @@
         <v>77</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="U17" t="s">
         <v>52</v>
@@ -2178,19 +2186,19 @@
         <v>52</v>
       </c>
       <c r="K18" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="M18" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="M18" s="2" t="s">
+      <c r="N18" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="N18" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="O18" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>77</v>
@@ -2199,10 +2207,10 @@
         <v>69</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="T18" s="2" t="s">
         <v>78</v>
@@ -2249,13 +2257,13 @@
         <v>96</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N19" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="O19" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>77</v>
@@ -2264,13 +2272,13 @@
         <v>98</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U19" t="s">
         <v>68</v>
@@ -2308,22 +2316,22 @@
         <v>95</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>79</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>78</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>98</v>
@@ -2373,19 +2381,19 @@
         <v>48.4</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>100</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>77</v>
@@ -2397,10 +2405,10 @@
         <v>83</v>
       </c>
       <c r="S21" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="T21" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="U21" t="s">
         <v>66</v>
@@ -2441,28 +2449,28 @@
         <v>83</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>77</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="T22" s="2" t="s">
         <v>98</v>
@@ -2503,10 +2511,10 @@
         <v>25.9</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>103</v>
@@ -2515,10 +2523,10 @@
         <v>75</v>
       </c>
       <c r="O23" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="P23" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="Q23" s="2" t="s">
         <v>77</v>
@@ -2565,19 +2573,19 @@
         <v>42.5</v>
       </c>
       <c r="K24" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="L24" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="M24" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>87</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P24" s="2" t="s">
         <v>77</v>
@@ -2589,7 +2597,7 @@
         <v>102</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="T24" s="2" t="s">
         <v>98</v>
@@ -2630,13 +2638,13 @@
         <v>25.5</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>87</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>98</v>
@@ -2648,13 +2656,13 @@
         <v>77</v>
       </c>
       <c r="Q25" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="R25" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="R25" s="2" t="s">
-        <v>176</v>
-      </c>
       <c r="S25" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T25" s="2" t="s">
         <v>76</v>
@@ -2707,16 +2715,16 @@
         <v>83</v>
       </c>
       <c r="P26" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q26" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="Q26" s="2" t="s">
-        <v>178</v>
-      </c>
       <c r="R26" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T26" s="2" t="s">
         <v>85</v>
@@ -2754,16 +2762,16 @@
         <v>54</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>87</v>
       </c>
       <c r="M27" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="N27" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="O27" s="2" t="s">
         <v>98</v>
@@ -2781,7 +2789,7 @@
         <v>79</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U27" t="s">
         <v>55</v>
@@ -2819,22 +2827,22 @@
         <v>24</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M28" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O28" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="N28" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="O28" s="2" t="s">
+      <c r="P28" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="Q28" s="2" t="s">
         <v>76</v>
@@ -2884,10 +2892,10 @@
         <v>99</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>96</v>
@@ -2899,13 +2907,13 @@
         <v>77</v>
       </c>
       <c r="Q29" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="R29" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="R29" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="S29" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T29" s="2" t="s">
         <v>85</v>
@@ -2946,16 +2954,16 @@
         <v>102</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M30" s="2" t="s">
         <v>78</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P30" s="2" t="s">
         <v>98</v>
@@ -2964,13 +2972,13 @@
         <v>77</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="S30" s="2" t="s">
         <v>87</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="U30" t="s">
         <v>54</v>
@@ -3014,10 +3022,10 @@
         <v>96</v>
       </c>
       <c r="N31" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="O31" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="P31" s="2" t="s">
         <v>98</v>
@@ -3029,10 +3037,10 @@
         <v>85</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T31" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U31" t="s">
         <v>55</v>
@@ -3070,16 +3078,16 @@
         <v>550</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>106</v>
       </c>
       <c r="M32" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="N32" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>195</v>
       </c>
       <c r="O32" s="2" t="s">
         <v>79</v>
@@ -3091,10 +3099,10 @@
         <v>81</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T32" s="2" t="s">
         <v>98</v>
@@ -3135,19 +3143,19 @@
         <v>162</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N33" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="O33" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="P33" s="2" t="s">
         <v>75</v>
@@ -3159,10 +3167,10 @@
         <v>97</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T33" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="U33" t="s">
         <v>61</v>
@@ -3197,13 +3205,13 @@
         <v>0.7</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N34" s="2" t="s">
         <v>80</v>
@@ -3211,8 +3219,8 @@
       <c r="O34" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="P34" s="2" t="s">
-        <v>175</v>
+      <c r="P34" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="Q34" s="2" t="s">
         <v>69</v>
@@ -3221,7 +3229,7 @@
         <v>77</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="T34" s="2" t="s">
         <v>98</v>
@@ -3262,16 +3270,16 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>100</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O35" s="2" t="s">
         <v>96</v>
@@ -3280,16 +3288,16 @@
         <v>83</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="S35" s="2" t="s">
         <v>98</v>
       </c>
       <c r="T35" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U35" t="s">
         <v>53</v>
@@ -3324,28 +3332,28 @@
         <v>36.5</v>
       </c>
       <c r="K36" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="L36" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="M36" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="N36" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="N36" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="O36" s="2" t="s">
         <v>96</v>
       </c>
       <c r="P36" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="R36" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="Q36" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="R36" s="2" t="s">
-        <v>207</v>
       </c>
       <c r="S36" s="2" t="s">
         <v>98</v>
@@ -3389,19 +3397,19 @@
         <v>69</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N37" s="2" t="s">
         <v>77</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q37" s="2" t="s">
         <v>99</v>
@@ -3410,10 +3418,10 @@
         <v>98</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="T37" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U37" t="s">
         <v>63</v>
@@ -3451,22 +3459,22 @@
         <v>20.100000000000001</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>83</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q38" s="2" t="s">
         <v>77</v>
@@ -3475,10 +3483,10 @@
         <v>69</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="T38" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="V38" t="s">
         <v>69</v>
@@ -3513,34 +3521,34 @@
         <v>22.2</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>98</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q39" s="2" t="s">
         <v>77</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="T39" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U39" t="s">
         <v>67</v>
@@ -3578,19 +3586,19 @@
         <v>52.2</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P40" s="2" t="s">
         <v>107</v>
@@ -3599,7 +3607,7 @@
         <v>79</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="S40" s="2" t="s">
         <v>98</v>
@@ -3640,25 +3648,25 @@
         <v>200.5</v>
       </c>
       <c r="K41" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="O41" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="N41" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="P41" s="2" t="s">
         <v>98</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="R41" s="2" t="s">
         <v>79</v>
@@ -3705,31 +3713,31 @@
         <v>63</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P42" s="2" t="s">
         <v>98</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="R42" s="2" t="s">
         <v>77</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T42" s="2" t="s">
         <v>85</v>
@@ -3770,19 +3778,19 @@
         <v>83</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>80</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q43" s="2" t="s">
         <v>98</v>
@@ -3791,7 +3799,7 @@
         <v>100</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="T43" s="2" t="s">
         <v>77</v>
@@ -3832,22 +3840,22 @@
         <v>23.5</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N44" s="2" t="s">
         <v>83</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q44" s="2" t="s">
         <v>98</v>
@@ -3859,7 +3867,7 @@
         <v>77</v>
       </c>
       <c r="T44" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="U44" t="s">
         <v>66</v>
@@ -3894,10 +3902,10 @@
         <v>38</v>
       </c>
       <c r="K45" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="L45" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>100</v>
@@ -3906,19 +3914,19 @@
         <v>83</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="R45" s="2" t="s">
         <v>96</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="T45" s="2" t="s">
         <v>85</v>
@@ -3959,34 +3967,34 @@
         <v>79.5</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>79</v>
       </c>
       <c r="M46" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q46" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="N46" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q46" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="R46" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S46" s="2" t="s">
         <v>97</v>
       </c>
       <c r="T46" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="U46" t="s">
         <v>59</v>
@@ -4021,13 +4029,13 @@
         <v>202</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>79</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N47" s="2" t="s">
         <v>102</v>
@@ -4039,10 +4047,10 @@
         <v>77</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="S47" s="2" t="s">
         <v>93</v>
@@ -4086,10 +4094,10 @@
         <v>27</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M48" s="2" t="s">
         <v>97</v>
@@ -4110,10 +4118,10 @@
         <v>69</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="T48" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="U48" t="s">
         <v>64</v>
@@ -4148,25 +4156,25 @@
         <v>29</v>
       </c>
       <c r="K49" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L49" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="M49" s="2" t="s">
         <v>75</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R49" s="2" t="s">
         <v>77</v>
@@ -4210,16 +4218,16 @@
         <v>100</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O50" s="2" t="s">
         <v>79</v>
@@ -4228,13 +4236,13 @@
         <v>98</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="T50" s="2" t="s">
         <v>85</v>
@@ -4275,7 +4283,7 @@
         <v>12</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>90</v>
@@ -4287,10 +4295,10 @@
         <v>83</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q51" s="2" t="s">
         <v>100</v>
@@ -4340,25 +4348,25 @@
         <v>51.5</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P52" s="2" t="s">
         <v>100</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="R52" s="2" t="s">
         <v>98</v>

</xml_diff>